<commit_message>
updated variable titles of workforce survey
</commit_message>
<xml_diff>
--- a/generator/data/generated_workers_variable_map.xlsx
+++ b/generator/data/generated_workers_variable_map.xlsx
@@ -498,7 +498,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Did you contract COVID-19?</t>
+          <t>Have you ever been infected by COVID-19?</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -586,7 +586,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Did your family members contract COVID-19?</t>
+          <t>Have any other family members been infected by COVID-19?</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -674,7 +674,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Did covid-19 cause your family to migrate to a different location?</t>
+          <t>Due to COVID-19, did your family have to migrate to a different location?</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -762,7 +762,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Did you suffer any of the following due to the economic downturn brought by covid-19?</t>
+          <t>Did you experience any of the following due to the economic downturn brought about by covid-19?</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -806,7 +806,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Due to COVID-19, did you face any of the following?</t>
+          <t>Due to have to any of the following due to COVID-19?</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -850,7 +850,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>When was the last time you received your full salary (or income)?</t>
+          <t>When was the last time you received your full salary (or full income)?</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>How many family members, including you, depended on your income before Covid-19</t>
+          <t>How many family members, including yourself, depended on your income before Covid-19?</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1158,7 +1158,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>How many family members, including you, depend on your income after Covid-19?</t>
+          <t>How many family members, including yourself, depend on your income after Covid-19?</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1202,7 +1202,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>How many of your family members’ basic needs can be met by your curret income?</t>
+          <t>How many of your family members’ basic needs can be met by your current income?</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1246,7 +1246,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>How much is your savings now compared to 2019?</t>
+          <t>Compared to the end of 2019, how much savings do you have now?</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -1290,7 +1290,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Which of the following facilities did your family have before Covid-19</t>
+          <t>Which of the following assets and amenities did your family have before Covid-19?</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1334,7 +1334,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Which of the following facilities does your family still have after Covid-19?</t>
+          <t>Which of the following assets and amenities does your family have after Covid-19?</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1378,7 +1378,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Do you owe any debt?</t>
+          <t>Do you have an outstanding debt?</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1422,7 +1422,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Did you learn any new skills when the tourism business was closed due to Covid-19?</t>
+          <t>Did you learn any new skills when the your tourism-related job/profession was halted due to Covid-19?</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1554,7 +1554,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Where did you get this training from?</t>
+          <t>Who provided this training?</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1598,7 +1598,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Which of the following sources do you use to get information about Covid-19?</t>
+          <t>Which of the following sources do you mainly use to get information about Covid-19? (Choose three main sources)</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1642,7 +1642,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Which of the following is suitable for you to reduce the effects caused by Covid-19?</t>
+          <t>Which of the following would help in reducing the effects of COVID-19 on you?</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1686,7 +1686,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>How long will the impact of Covid-19 on your livelihood last?</t>
+          <t>How much longer will COVID-19 affect your livelihood? Provide your best estimate.</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1730,7 +1730,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>How long will it take for your employment to return to normal after the tourism sector is up and running?</t>
+          <t>How long will it take for your employment to return to normal after the tourism sector is up and running again? Provide your best estimate.</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1774,7 +1774,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>If this situation continues for the next 6 months, which of the following conditions will you have to face?</t>
+          <t>If the current situation continues for the next 6 months, which of the following difficulties will you face?</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1818,7 +1818,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Do you have any collateral/securities required to get additional loan?</t>
+          <t>Do you have the necessary collateral/securities to secure additional loans?</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1862,7 +1862,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>What are the major challenges for the revival of the tourism sector you are involved in?</t>
+          <t>What are the major challenges for the revival of the tourism sub-sector you are involved in?</t>
         </is>
       </c>
       <c r="D33" t="n">

</xml_diff>

<commit_message>
Updated charts data for businesses
</commit_message>
<xml_diff>
--- a/generator/data/generated_workers_variable_map.xlsx
+++ b/generator/data/generated_workers_variable_map.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,36 +503,36 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>i_lvlhd_domicile_chng_self_fml</t>
+          <t>n_rcvry_preferred_empl_incentives</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>कोभिड-१९ को कारणले के तपाईंं आफु बस्दै आएको ठाउँ परिवर्तन गर्नुपर्यो?</t>
+          <t>कोभिड-१९ ले पारेको असर कम गर्न तपाईंँलाई निम्न मध्ये कुन-कुन रोजगार सम्बन्धि सहयोगहरु उपयुक्त हुन्छन् ?</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Due to COVID-19, did you have to migrate to a different location?</t>
+          <t>Which of the following employment related support would help in reducing the effects of COVID-19 on you?</t>
         </is>
       </c>
       <c r="D2" t="n">
         <v>258</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>single-select</t>
+          <t>multi-select</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>impact</t>
+          <t>need</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -542,12 +542,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Impact on livelihood</t>
+          <t>Assistance</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>More then 55% had to relocate</t>
+          <t>What kind of support will be useful?</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -562,24 +562,24 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>i_empl_jb_prsnt_status</t>
+          <t>i_lvlhd_domicile_chng_self_fml</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>के तपाईंं अझै पर्यटन क्षेत्रमै काम गर्दै हुनुहुन्छ ?</t>
+          <t>कोभिड-१९ को कारणले के तपाईंं आफु बस्दै आएको ठाउँ परिवर्तन गर्नुपर्यो?</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Are you still working in the tourism sector?</t>
+          <t>Due to COVID-19, did you have to migrate to a different location?</t>
         </is>
       </c>
       <c r="D3" t="n">
         <v>258</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
@@ -606,7 +606,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>More then 80% lost job</t>
+          <t>More then 55% had to relocate</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -621,31 +621,31 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>i_empl_covid_effects</t>
+          <t>i_empl_jb_prsnt_status</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>कोभिड-१९ ले ल्याएको आर्थिक मन्दीका कारणले गर्दा के तपाईंंले निम्न मध्ये कुनै भोग्नुपर्यो?</t>
+          <t>के तपाईंं अझै पर्यटन क्षेत्रमै काम गर्दै हुनुहुन्छ ?</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Did you experience any of the following due to the economic downturn brought about by covid-19?</t>
+          <t>Are you still working in the tourism sector?</t>
         </is>
       </c>
       <c r="D4" t="n">
         <v>258</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>multi-select</t>
+          <t>single-select</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -665,7 +665,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>More then 70% left unemployed</t>
+          <t>More then 80% lost job</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -680,31 +680,31 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>i_econ_incm_chng_self</t>
+          <t>i_empl_covid_effects</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>सन् २०१९ को तुलनामा सन् २०२० मा तपाईंंको कुल आय कसरी परिवर्तन भयो?</t>
+          <t>कोभिड-१९ ले ल्याएको आर्थिक मन्दीका कारणले गर्दा के तपाईंंले निम्न मध्ये कुनै भोग्नुपर्यो?</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>How did your total income change in 2020 compared to 2019?</t>
+          <t>Did you experience any of the following due to the economic downturn brought about by covid-19?</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>258</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>single-select</t>
+          <t>multi-select</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -719,17 +719,17 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Impact on finance</t>
+          <t>Impact on livelihood</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Of those employed, two-thirds earning less than before the pandemic</t>
+          <t>More then 70% left unemployed</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>value</t>
+          <t>percentage</t>
         </is>
       </c>
       <c r="M5" t="n">
@@ -739,24 +739,24 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>i_empl_lst_date_full_salary</t>
+          <t>i_econ_incm_chng_self</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>पछिल्लो पल्ट आफ्नो पूर्ण तलब (वा आम्दानी) पाउनुभएको कति भयो?</t>
+          <t>सन् २०१९ को तुलनामा सन् २०२० मा तपाईंंको कुल आय कसरी परिवर्तन भयो?</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>When was the last time you received your full salary (or full income)?</t>
+          <t>How did your total income change in 2020 compared to 2019?</t>
         </is>
       </c>
       <c r="D6" t="n">
         <v>258</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
@@ -783,7 +783,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>More than 14 months since having received full income</t>
+          <t>Of those employed, two-thirds earning less than before the pandemic</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -798,24 +798,24 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>p_econ_self_savings_chng_today_v_19</t>
+          <t>i_empl_lst_date_full_salary</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>सन् २०१९ को तुलनामा तपाईंँको बचत अहिले कति बाँकी रहेको छ ?</t>
+          <t>पछिल्लो पल्ट आफ्नो पूर्ण तलब (वा आम्दानी) पाउनुभएको कति भयो?</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Compared to the end of 2019, how much savings do you have now?</t>
+          <t>When was the last time you received your full salary (or full income)?</t>
         </is>
       </c>
       <c r="D7" t="n">
         <v>258</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
@@ -842,7 +842,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Savings reduced to near zero for more than 90% of respondents</t>
+          <t>More than 14 months since having received full income</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -857,24 +857,24 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>p_lvlhd_num_depndnt_fml_membrs_post_covid</t>
+          <t>p_econ_self_savings_chng_today_v_19</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>कोभिड-१९ भन्दा पछी तपाईंँको आयमा तपाईंँ लगायत कति जना परिवार सदस्यहरू निर्भर छन् ?</t>
+          <t>सन् २०१९ को तुलनामा तपाईंँको बचत अहिले कति बाँकी रहेको छ ?</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>How many family members, including yourself, depend on your income after Covid-19?</t>
+          <t>Compared to the end of 2019, how much savings do you have now?</t>
         </is>
       </c>
       <c r="D8" t="n">
         <v>258</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
@@ -901,7 +901,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Most of them have more than 3 people to look after, but...</t>
+          <t>Savings reduced to near zero for more than 90% of respondents</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -916,24 +916,24 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>p_lvlhd_num_depndnt_need_fml_membrs_post_covid</t>
+          <t>p_lvlhd_num_depndnt_fml_membrs_post_covid</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>तपाईंँको हालको आय कति जना परिवार सदस्यको आधारभूत आवश्यकता पूर्ति गर्न पर्याप्त छ ?</t>
+          <t>कोभिड-१९ भन्दा पछी तपाईंँको आयमा तपाईंँ लगायत कति जना परिवार सदस्यहरू निर्भर छन् ?</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>How many of your family members’ basic needs can be met by your current income?</t>
+          <t>How many family members, including yourself, depend on your income after Covid-19?</t>
         </is>
       </c>
       <c r="D9" t="n">
         <v>258</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>1</v>
@@ -960,7 +960,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>... income is not even sufficient for themselves</t>
+          <t>Most of them have more than 3 people to look after, but...</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -975,24 +975,24 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>p_econ_outstndng_loans_self</t>
+          <t>p_lvlhd_num_depndnt_need_fml_membrs_post_covid</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>के तपाईंँको कुनै ऋण तिर्न बाँकी छ ?</t>
+          <t>तपाईंँको हालको आय कति जना परिवार सदस्यको आधारभूत आवश्यकता पूर्ति गर्न पर्याप्त छ ?</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Do you have an outstanding debt?</t>
+          <t>How many of your family members’ basic needs can be met by your current income?</t>
         </is>
       </c>
       <c r="D10" t="n">
         <v>258</v>
       </c>
       <c r="E10" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" t="n">
         <v>1</v>
@@ -1019,12 +1019,12 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Trouble ahead: 92% are already in some kind of debt</t>
+          <t>... income is not even sufficient for themselves</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>percentage</t>
+          <t>value</t>
         </is>
       </c>
       <c r="M10" t="n">
@@ -1034,24 +1034,24 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>i_hlth_covid_infectn_self_fml</t>
+          <t>p_econ_outstndng_loans_self</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>के तपाईंँको परिवारमा कसैलाई कोभिड-१९ लागेको छ/थियो?</t>
+          <t>के तपाईंँको कुनै ऋण तिर्न बाँकी छ ?</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Have any one in your family ever been infected by COVID-19?</t>
+          <t>Do you have an outstanding debt?</t>
         </is>
       </c>
       <c r="D11" t="n">
         <v>258</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
         <v>1</v>
@@ -1073,17 +1073,17 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Impact on health</t>
+          <t>Impact on finance</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Avoided  COVID-19 infection...</t>
+          <t>Trouble ahead: 92% are already in some kind of debt</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>value</t>
+          <t>percentage</t>
         </is>
       </c>
       <c r="M11" t="n">
@@ -1093,31 +1093,31 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>i_mental_hlth</t>
+          <t>i_hlth_covid_infectn_self_fml</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>कोभिड-१९ to को कारणले गर्दा तपाईंले निम्न मध्ये कुनै पनि मनोवैज्ञानिक प्रभावहरू भोग्नुभयो?</t>
+          <t>के तपाईंँको परिवारमा कसैलाई कोभिड-१९ लागेको छ/थियो?</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Did you suffer any of the following psychosocial impact due to covid-19?</t>
+          <t>Have any one in your family ever been infected by COVID-19?</t>
         </is>
       </c>
       <c r="D12" t="n">
         <v>258</v>
       </c>
       <c r="E12" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
         <v>1</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>multi-select</t>
+          <t>single-select</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1137,12 +1137,12 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>But, couldn't avoid psycho-social impact, About 95% reported some sort of psycho-social impact</t>
+          <t>Avoided  COVID-19 infection...</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>percentage</t>
+          <t>value</t>
         </is>
       </c>
       <c r="M12" t="n">
@@ -1152,36 +1152,36 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>p_econ_altrnt_incm_src_self_fml_flg</t>
+          <t>i_mental_hlth</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>तपाईंं अथवा तपाईंँको परिवारको पर्यटन बाहेक वैकल्पिक आय श्रोत छ?</t>
+          <t>कोभिड-१९ to को कारणले गर्दा तपाईंले निम्न मध्ये कुनै पनि मनोवैज्ञानिक प्रभावहरू भोग्नुभयो?</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Do you or your family have an alternative source of income other than tourism?</t>
+          <t>Did you suffer any of the following psycho-social impact due to covid-19?</t>
         </is>
       </c>
       <c r="D13" t="n">
         <v>258</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>single-select</t>
+          <t>multi-select</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>preparedness</t>
+          <t>impact</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1191,17 +1191,17 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Coping mechanism</t>
+          <t>Impact on health</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Alternative income source but more than 80%  are dependent on tourism sector only. (i.e. they don't have alternative source of income)</t>
+          <t>But, couldn't avoid psycho-social impact, About 95% reported some sort of psycho-social impact</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>value</t>
+          <t>percentage</t>
         </is>
       </c>
       <c r="M13" t="n">
@@ -1211,31 +1211,31 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>i_econ_covid_effects_fin</t>
+          <t>p_econ_altrnt_incm_src_self_fml_flg</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>कोभिड-१९ को कारणले गर्दा के तपाईंंले निम्न मध्ये कुनै भोग्नु/गर्नु पर्यो?</t>
+          <t>तपाईंं अथवा तपाईंँको परिवारको पर्यटन बाहेक वैकल्पिक आय श्रोत छ?</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Which of the following loan related actions did you have to take due to the pandemic?</t>
+          <t>Do you or your family have an alternative source of income other than tourism?</t>
         </is>
       </c>
       <c r="D14" t="n">
         <v>258</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>multi-select</t>
+          <t>single-select</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1255,12 +1255,12 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Around 80% have borrowed money, but few did so through financial institutions</t>
+          <t>Alternative income source but more than 80%  are dependent on tourism sector only. (i.e. they don't have alternative source of income)</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>percentage</t>
+          <t>value</t>
         </is>
       </c>
       <c r="M14" t="n">
@@ -1270,20 +1270,24 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>i_econ_covid_effects_assets</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
+          <t>i_econ_covid_effects_fin</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>कोभिड-१९ को कारणले गर्दा के तपाईंंले निम्न मध्ये कुनै ऋण सम्बन्धित प्रभावहरू भोग्नु/गर्नु पर्यो?</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Which of the following assets related actions did you have to take due to the pandemic?</t>
+          <t>Which of the following loan related actions did you have to take due to the pandemic?</t>
         </is>
       </c>
       <c r="D15" t="n">
         <v>258</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
         <v>1</v>
@@ -1310,7 +1314,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>One in four persons have had to sell their assets</t>
+          <t>Around 80% have borrowed money, but few did so through financial institutions</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1325,20 +1329,24 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>i_econ_covid_effects_services</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
+          <t>i_econ_covid_effects_assets</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>कोभिड-१९ को कारणले गर्दा के तपाईंंले निम्न मध्ये कुनै सम्पत्ति सम्बन्धित असर भोग्नु/गर्नु पर्यो?</t>
+        </is>
+      </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Which of the following family services related actions did you have to take due to the pandemic?</t>
+          <t>Which of the following assets related actions did you have to take due to the pandemic?</t>
         </is>
       </c>
       <c r="D16" t="n">
         <v>258</v>
       </c>
       <c r="E16" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16" t="n">
         <v>1</v>
@@ -1365,7 +1373,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Stopped health and education services of family members</t>
+          <t>One in four persons have had to sell their assets</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1380,31 +1388,31 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>p_hlth_vaccinated_self</t>
+          <t>i_econ_covid_effects_services</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>के तपाईंँले कोभिड-१९ को खोप लगाउनुभएको छ ?</t>
+          <t>कोभिड-१९ को कारणले गर्दा के तपाईंंले निम्न मध्ये कुनै पारिवारिक सेवाहरूमा असर भोग्नु/गर्नु पर्यो?</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Have you been vaccinated against Covid-19?</t>
+          <t>Which of the following family services related actions did you have to take due to the pandemic?</t>
         </is>
       </c>
       <c r="D17" t="n">
         <v>258</v>
       </c>
       <c r="E17" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F17" t="n">
         <v>1</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>single-select</t>
+          <t>multi-select</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1419,17 +1427,17 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Health and saftey actions</t>
+          <t>Coping mechanism</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Nearly half of the respondents reported to be vaccinated against COVID-19</t>
+          <t>Stopped health and education services of family members</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>value</t>
+          <t>percentage</t>
         </is>
       </c>
       <c r="M17" t="n">
@@ -1439,24 +1447,24 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>p_hlth_received_hhs_training_self</t>
+          <t>p_hlth_vaccinated_self</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>के तपाईंँले कोभिड-१९ सम्बन्धी स्वास्थ्य तथा सुरक्षाको तालिम प्राप्त गर्नुभएको छ ?</t>
+          <t>के तपाईंँले कोभिड-१९ को खोप लगाउनुभएको छ ?</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Have you received any health and safety training related to Covid-19?</t>
+          <t>Have you been vaccinated against Covid-19?</t>
         </is>
       </c>
       <c r="D18" t="n">
         <v>258</v>
       </c>
       <c r="E18" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18" t="n">
         <v>1</v>
@@ -1478,12 +1486,12 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Health and saftey</t>
+          <t>Health and saftey actions</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Health and safety training, More than 95% didn't receive health and saftey related training</t>
+          <t>Nearly half of the respondents reported to be vaccinated against COVID-19</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1498,24 +1506,24 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>i_mental_hlth_therapy</t>
+          <t>p_hlth_received_hhs_training_self</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>कोभिड-१९ले ल्याएको मानसिक तनावको लागि कुनै किसिमको स्वास्थ्य परामर्श सेवा लिनुभएको छ?</t>
+          <t>के तपाईंँले कोभिड-१९ सम्बन्धी स्वास्थ्य तथा सुरक्षाको तालिम प्राप्त गर्नुभएको छ ?</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Have you taken any kind of health counseling service for the mental stress brought by Covid-19?</t>
+          <t>Have you received any health and safety training related to Covid-19?</t>
         </is>
       </c>
       <c r="D19" t="n">
         <v>258</v>
       </c>
       <c r="E19" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F19" t="n">
         <v>1</v>
@@ -1542,7 +1550,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Even if 95% reported some sorted of psycho-social impact, only 13% seeked for help</t>
+          <t>Health and safety training, More than 95% didn't receive health and saftey related training</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1557,31 +1565,31 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>p_hlth_info_covid_src</t>
+          <t>i_mental_hlth_therapy</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>कोभिड-१९ को बारेमा जानकारी पाउन निम्न मध्ये कुन-कुन स्रोतहरू प्रयोग गर्नुहुन्छ? (मुख्य तीनवटा छान्नुहोस्)</t>
+          <t>कोभिड-१९ले ल्याएको मानसिक तनावको लागि कुनै किसिमको स्वास्थ्य परामर्श सेवा लिनुभएको छ?</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Which of the following sources do you mainly use to get information about Covid-19? (Choose three main sources)</t>
+          <t>Have you taken any kind of health counseling service for the mental stress brought by Covid-19?</t>
         </is>
       </c>
       <c r="D20" t="n">
         <v>258</v>
       </c>
       <c r="E20" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F20" t="n">
         <v>1</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>multi-select</t>
+          <t>single-select</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1601,12 +1609,12 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Getting informed about COVID-19, Social-Media on the top</t>
+          <t>Even if 95% reported some sorted of psycho-social impact, only 13% seeked for help</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>percentage</t>
+          <t>value</t>
         </is>
       </c>
       <c r="M20" t="n">
@@ -1616,24 +1624,24 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>n_rcvry_preferred_incentives</t>
+          <t>p_hlth_info_covid_src</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>कोभिड-१९ ले पारेको असर कम गर्न तपाईंँलाई निम्न मध्ये कुन-कुन उपयुक्त हुन्छन् ?</t>
+          <t>कोभिड-१९ को बारेमा जानकारी पाउन निम्न मध्ये कुन-कुन स्रोतहरू प्रयोग गर्नुहुन्छ? (मुख्य तीनवटा छान्नुहोस्)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Which of the following would help in reducing the effects of COVID-19 on you?</t>
+          <t>Which of the following sources do you mainly use to get information about Covid-19? (Choose three main sources)</t>
         </is>
       </c>
       <c r="D21" t="n">
         <v>258</v>
       </c>
       <c r="E21" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F21" t="n">
         <v>1</v>
@@ -1645,7 +1653,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>need</t>
+          <t>preparedness</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1655,12 +1663,12 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Assistance</t>
+          <t>Health and saftey</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>What kind of support will be useful?</t>
+          <t>Getting informed about COVID-19, Social-Media on the top</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -1675,36 +1683,36 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>o_econ_impact_how_long_months</t>
+          <t>n_rcvry_preferred_fin_incentives</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>कोभिड-१९ ले तपाईंंको जिविकोपार्जनमा पारेको असर अझै कति समय सम्म रहला जस्तो छ ?</t>
+          <t>कोभिड-१९ ले पारेको असर कम गर्न तपाईंँलाई निम्न मध्ये कुन-कुन आर्थिक सहयोगहरु उपयुक्त हुन्छन् ?</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>For how much longer do you expect the effect of the pandemic on your livelihood to last?</t>
+          <t>Which of the following financial support would help in reducing the effects of COVID-19 on you?</t>
         </is>
       </c>
       <c r="D22" t="n">
         <v>258</v>
       </c>
       <c r="E22" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F22" t="n">
         <v>1</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>single-select</t>
+          <t>multi-select</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>outlook</t>
+          <t>need</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1714,13 +1722,17 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Workforce perception check</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr"/>
+          <t>Assistance</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>What kind of support will be useful?</t>
+        </is>
+      </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>value</t>
+          <t>percentage</t>
         </is>
       </c>
       <c r="M22" t="n">
@@ -1730,24 +1742,24 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>o_empl_status_to_nrml_how_long_months</t>
+          <t>o_econ_impact_how_long_months</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>पर्यटन क्षेत्र सुचारु भएपश्चात आफ्नो रोजगार पहिलेको जस्तो अवस्थामा पुर्याउन कति समय लाग्ला?</t>
+          <t>कोभिड-१९ ले तपाईंंको जिविकोपार्जनमा पारेको असर अझै कति समय सम्म रहला जस्तो छ ?</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>How long will it take for your employment to return to normal after the tourism sector is up and running again? Provide your best estimate.</t>
+          <t>For how much longer do you expect the effect of the pandemic on your livelihood to last?</t>
         </is>
       </c>
       <c r="D23" t="n">
         <v>258</v>
       </c>
       <c r="E23" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F23" t="n">
         <v>1</v>
@@ -1785,31 +1797,31 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>o_impct_to_self_nxt_6_mnths</t>
+          <t>o_empl_status_to_nrml_how_long_months</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>आउँदो ६ महिना सम्म यही परिस्थिति रहेमा निम्नमध्ये कुन-कुन अवस्था तपाईंंले भोग्नु पर्ने हुन्छ?</t>
+          <t>पर्यटन क्षेत्र सुचारु भएपश्चात आफ्नो रोजगार पहिलेको जस्तो अवस्थामा पुर्याउन कति समय लाग्ला?</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>If the current situation continues for the next 6 months, which of the following difficulties will you face?</t>
+          <t>How long will it take for your employment to return to normal after the tourism sector is up and running again? Provide your best estimate.</t>
         </is>
       </c>
       <c r="D24" t="n">
         <v>258</v>
       </c>
       <c r="E24" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F24" t="n">
         <v>1</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>multi-select</t>
+          <t>single-select</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1827,14 +1839,10 @@
           <t>Workforce perception check</t>
         </is>
       </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>Expected difficulties in the next six months</t>
-        </is>
-      </c>
+      <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr">
         <is>
-          <t>percentage</t>
+          <t>value</t>
         </is>
       </c>
       <c r="M24" t="n">
@@ -1844,24 +1852,24 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>o_rcvry_chllng_trsm_revival</t>
+          <t>o_impct_to_self_nxt_6_mnths</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>तपाईंं संलग्न रहेको पर्यटन क्षेत्रको पुन:उत्थानको निम्ति प्रमुख चुनौतीहरू के-के छन् ?</t>
+          <t>आउँदो ६ महिना सम्म यही परिस्थिति रहेमा निम्नमध्ये कुन-कुन अवस्था तपाईंंले भोग्नु पर्ने हुन्छ?</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>What are the major challenges for the revival of the tourism sub-sector you are involved in?</t>
+          <t>If the current situation continues for the next 6 months, which of the following difficulties will you face?</t>
         </is>
       </c>
       <c r="D25" t="n">
         <v>258</v>
       </c>
       <c r="E25" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F25" t="n">
         <v>1</v>
@@ -1888,7 +1896,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Biggest challenges of Nepali tourism: what do the workers think?</t>
+          <t>Expected difficulties in the next six months</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -1903,31 +1911,31 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>o_econ_impact_fml_income_chng_21_v_19</t>
+          <t>o_rcvry_chllng_trsm_revival</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>सन् २०१९ को तुलनामा सन् २०२१ मा तपाईंंको परिवारको आय कति रहने अनुमान छ?</t>
+          <t>तपाईंं संलग्न रहेको पर्यटन क्षेत्रको पुन:उत्थानको निम्ति प्रमुख चुनौतीहरू के-के छन् ?</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>What is the estimated income of your family in 2021 compared to 2019?</t>
+          <t>What are the major challenges for the revival of the tourism sub-sector you are involved in?</t>
         </is>
       </c>
       <c r="D26" t="n">
         <v>258</v>
       </c>
       <c r="E26" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F26" t="n">
         <v>1</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>single-select</t>
+          <t>multi-select</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1947,12 +1955,12 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Estimated income for 2021</t>
+          <t>Biggest challenges of Nepali tourism: what do the workers think?</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>value</t>
+          <t>percentage</t>
         </is>
       </c>
       <c r="M26" t="n">
@@ -1962,34 +1970,38 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>m_gender</t>
+          <t>o_econ_impact_fml_income_chng_21_v_19</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>लिङ्ग</t>
+          <t>सन् २०१९ को तुलनामा सन् २०२१ मा तपाईंंको परिवारको आय कति रहने अनुमान छ?</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>What is the estimated income of your family in 2021 compared to 2019?</t>
         </is>
       </c>
       <c r="D27" t="n">
         <v>258</v>
       </c>
       <c r="E27" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F27" t="n">
         <v>1</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>groupby</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr"/>
+          <t>single-select</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>outlook</t>
+        </is>
+      </c>
       <c r="I27" t="inlineStr">
         <is>
           <t>general</t>
@@ -1997,10 +2009,14 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>general</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr"/>
+          <t>Workforce perception check</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Estimated income for 2021</t>
+        </is>
+      </c>
       <c r="L27" t="inlineStr">
         <is>
           <t>value</t>
@@ -2013,24 +2029,24 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>m_age</t>
+          <t>m_gender</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>उमेर</t>
+          <t>लिङ्ग</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Age</t>
+          <t>Gender</t>
         </is>
       </c>
       <c r="D28" t="n">
         <v>258</v>
       </c>
       <c r="E28" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F28" t="n">
         <v>1</v>
@@ -2064,24 +2080,24 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>m_edu_levl</t>
+          <t>m_age</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>पूरा गरेको शैक्षिक तह</t>
+          <t>उमेर</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Completed educational level</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="D29" t="n">
         <v>258</v>
       </c>
       <c r="E29" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F29" t="n">
         <v>1</v>
@@ -2115,24 +2131,24 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>m_years_of_experience</t>
+          <t>m_edu_levl</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>तपाईंँ पर्यटन क्षेत्रमा काम गर्नुभएको कति समय भयो?</t>
+          <t>पूरा गरेको शैक्षिक तह</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>How long have you been working in the tourism sector?</t>
+          <t>Completed educational level</t>
         </is>
       </c>
       <c r="D30" t="n">
         <v>258</v>
       </c>
       <c r="E30" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F30" t="n">
         <v>1</v>
@@ -2160,6 +2176,57 @@
         </is>
       </c>
       <c r="M30" t="n">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>m_years_of_experience</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>तपाईंँ पर्यटन क्षेत्रमा काम गर्नुभएको कति समय भयो?</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>How long have you been working in the tourism sector?</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>258</v>
+      </c>
+      <c r="E31" t="n">
+        <v>29</v>
+      </c>
+      <c r="F31" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>groupby</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>general</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>general</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="M31" t="n">
         <v>258</v>
       </c>
     </row>

</xml_diff>